<commit_message>
Changes of MNX Track
</commit_message>
<xml_diff>
--- a/src/main/resources/MNX_PROD.xlsx
+++ b/src/main/resources/MNX_PROD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Local\MNX Tracking\MNXTracking\src\main\resources\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
   <si>
     <t>Account</t>
   </si>
@@ -251,12 +251,52 @@
   </si>
   <si>
     <t>34769</t>
+  </si>
+  <si>
+    <t>15590849</t>
+  </si>
+  <si>
+    <t>15590965</t>
+  </si>
+  <si>
+    <t>15590968</t>
+  </si>
+  <si>
+    <t>11189259</t>
+  </si>
+  <si>
+    <t>7391135</t>
+  </si>
+  <si>
+    <t>15591265</t>
+  </si>
+  <si>
+    <t>15591285</t>
+  </si>
+  <si>
+    <t>15591316</t>
+  </si>
+  <si>
+    <t>11189341</t>
+  </si>
+  <si>
+    <t>7391186</t>
+  </si>
+  <si>
+    <t>15592291</t>
+  </si>
+  <si>
+    <t>11189676</t>
+  </si>
+  <si>
+    <t>7391426</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -682,45 +722,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="7.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="13.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="17.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="18.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="18.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="13.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="9.140625" style="1" collapsed="1"/>
-    <col min="36" max="36" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="9.140625" style="1" collapsed="1"/>
-    <col min="38" max="38" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="15.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="33.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="17.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="8.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="9" width="17.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="21.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="1" width="13.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="1" width="16.140625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="2" width="18.140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="1" width="18.140625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="13.5703125" collapsed="true"/>
+    <col min="35" max="35" style="1" width="9.140625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="37" max="37" style="1" width="9.140625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
+    <col min="39" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="8" customFormat="1">
@@ -787,10 +827,10 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>10</v>
@@ -1050,7 +1090,7 @@
         <v>73</v>
       </c>
       <c r="AG2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="AH2" s="7"/>
       <c r="AI2" t="s">

</xml_diff>

<commit_message>
Changes of MNX tracking final
</commit_message>
<xml_diff>
--- a/src/main/resources/MNX_PROD.xlsx
+++ b/src/main/resources/MNX_PROD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="114">
   <si>
     <t>Account</t>
   </si>
@@ -290,6 +290,78 @@
   </si>
   <si>
     <t>7391426</t>
+  </si>
+  <si>
+    <t>15594943</t>
+  </si>
+  <si>
+    <t>11190950</t>
+  </si>
+  <si>
+    <t>7392332</t>
+  </si>
+  <si>
+    <t>15594985</t>
+  </si>
+  <si>
+    <t>11190976</t>
+  </si>
+  <si>
+    <t>7392353</t>
+  </si>
+  <si>
+    <t>15595042</t>
+  </si>
+  <si>
+    <t>11191003</t>
+  </si>
+  <si>
+    <t>7392365</t>
+  </si>
+  <si>
+    <t>15595065</t>
+  </si>
+  <si>
+    <t>11191011</t>
+  </si>
+  <si>
+    <t>7392376</t>
+  </si>
+  <si>
+    <t>15595085</t>
+  </si>
+  <si>
+    <t>11191026</t>
+  </si>
+  <si>
+    <t>7392390</t>
+  </si>
+  <si>
+    <t>15595111</t>
+  </si>
+  <si>
+    <t>11191050</t>
+  </si>
+  <si>
+    <t>7392405</t>
+  </si>
+  <si>
+    <t>15595120</t>
+  </si>
+  <si>
+    <t>11191056</t>
+  </si>
+  <si>
+    <t>7392412</t>
+  </si>
+  <si>
+    <t>15595151</t>
+  </si>
+  <si>
+    <t>11191070</t>
+  </si>
+  <si>
+    <t>7392424</t>
   </si>
 </sst>
 </file>
@@ -827,10 +899,10 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>10</v>
@@ -1090,7 +1162,7 @@
         <v>73</v>
       </c>
       <c r="AG2" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="AH2" s="7"/>
       <c r="AI2" t="s">

</xml_diff>

<commit_message>
Changess of reports and screenshots
</commit_message>
<xml_diff>
--- a/src/main/resources/MNX_PROD.xlsx
+++ b/src/main/resources/MNX_PROD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="117">
   <si>
     <t>Account</t>
   </si>
@@ -362,6 +362,15 @@
   </si>
   <si>
     <t>7392424</t>
+  </si>
+  <si>
+    <t>15595207</t>
+  </si>
+  <si>
+    <t>11191100</t>
+  </si>
+  <si>
+    <t>7392452</t>
   </si>
 </sst>
 </file>
@@ -899,10 +908,10 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>10</v>
@@ -1162,7 +1171,7 @@
         <v>73</v>
       </c>
       <c r="AG2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AH2" s="7"/>
       <c r="AI2" t="s">

</xml_diff>